<commit_message>
fix hainan area unit
</commit_message>
<xml_diff>
--- a/src/main/resources/data/hainan/天然橡胶.xlsx
+++ b/src/main/resources/data/hainan/天然橡胶.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="27945" windowHeight="12375" tabRatio="826" firstSheet="2" activeTab="8"/>
+    <workbookView windowWidth="24045" windowHeight="12375" tabRatio="826" firstSheet="3" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="左1-近年海南天然橡胶面积" sheetId="2" r:id="rId1"/>
@@ -41,14 +41,14 @@
   </si>
   <si>
     <t xml:space="preserve">年末面积
-(公顷)
+(万亩)
 </t>
   </si>
   <si>
-    <t>新种面积(公顷)</t>
-  </si>
-  <si>
-    <t>收获面积(公顷)</t>
+    <t>新种面积(万亩)</t>
+  </si>
+  <si>
+    <t>收获面积(万亩)</t>
   </si>
   <si>
     <t xml:space="preserve">总产量(吨）
@@ -3749,7 +3749,7 @@
     <t>市县</t>
   </si>
   <si>
-    <t>2022年年末面积(公顷)</t>
+    <t>2022年年末面积(万亩)</t>
   </si>
   <si>
     <t>2022年总产量(吨）</t>
@@ -3805,7 +3805,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="176" formatCode="0.00_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -3852,6 +3852,19 @@
     <font>
       <sz val="10.5"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10.5"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
     </font>
@@ -4404,137 +4417,137 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -4629,6 +4642,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="8" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -4953,7 +4978,7 @@
   <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="3"/>
@@ -4964,87 +4989,87 @@
   </cols>
   <sheetData>
     <row r="1" ht="44.25" spans="1:4">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="32" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="33" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="21" t="s">
+      <c r="C1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" ht="15.75" spans="1:4">
-      <c r="A2" s="23">
+      <c r="A2" s="35">
         <v>2018</v>
       </c>
-      <c r="B2" s="28">
-        <v>528351</v>
-      </c>
-      <c r="C2" s="28">
-        <v>8008</v>
-      </c>
-      <c r="D2" s="28">
-        <v>381113</v>
+      <c r="B2" s="35">
+        <v>792.5265</v>
+      </c>
+      <c r="C2" s="35">
+        <v>12.012</v>
+      </c>
+      <c r="D2" s="35">
+        <v>571.6695</v>
       </c>
     </row>
     <row r="3" ht="15.75" spans="1:4">
-      <c r="A3" s="23">
+      <c r="A3" s="35">
         <v>2019</v>
       </c>
-      <c r="B3" s="28">
-        <v>526897</v>
-      </c>
-      <c r="C3" s="23">
-        <v>3870</v>
-      </c>
-      <c r="D3" s="28">
-        <v>381301</v>
+      <c r="B3" s="35">
+        <v>790.3455</v>
+      </c>
+      <c r="C3" s="35">
+        <v>5.805</v>
+      </c>
+      <c r="D3" s="35">
+        <v>571.9515</v>
       </c>
     </row>
     <row r="4" ht="15.75" spans="1:4">
-      <c r="A4" s="23">
+      <c r="A4" s="35">
         <v>2020</v>
       </c>
-      <c r="B4" s="28">
-        <v>519184</v>
-      </c>
-      <c r="C4" s="23">
-        <v>3453</v>
-      </c>
-      <c r="D4" s="28">
-        <v>394444</v>
+      <c r="B4" s="35">
+        <v>778.776</v>
+      </c>
+      <c r="C4" s="35">
+        <v>5.1795</v>
+      </c>
+      <c r="D4" s="35">
+        <v>591.666</v>
       </c>
     </row>
     <row r="5" ht="15.75" spans="1:4">
-      <c r="A5" s="23">
+      <c r="A5" s="35">
         <v>2021</v>
       </c>
-      <c r="B5" s="28">
-        <v>512613</v>
-      </c>
-      <c r="C5" s="23">
-        <v>7327</v>
-      </c>
-      <c r="D5" s="28">
-        <v>404327</v>
+      <c r="B5" s="35">
+        <v>768.9195</v>
+      </c>
+      <c r="C5" s="35">
+        <v>10.9905</v>
+      </c>
+      <c r="D5" s="35">
+        <v>606.4905</v>
       </c>
     </row>
     <row r="6" ht="15.75" spans="1:4">
-      <c r="A6" s="23">
+      <c r="A6" s="35">
         <v>2022</v>
       </c>
-      <c r="B6" s="28">
-        <v>518590</v>
-      </c>
-      <c r="C6" s="23">
-        <v>3037</v>
-      </c>
-      <c r="D6" s="28">
-        <v>396032</v>
+      <c r="B6" s="35">
+        <v>777.885</v>
+      </c>
+      <c r="C6" s="35">
+        <v>4.5555</v>
+      </c>
+      <c r="D6" s="35">
+        <v>594.048</v>
       </c>
     </row>
     <row r="7" ht="15"/>
@@ -18697,8 +18722,8 @@
   <sheetPr/>
   <dimension ref="A1:C19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="2"/>
@@ -18724,7 +18749,7 @@
         <v>88</v>
       </c>
       <c r="B2" s="16">
-        <v>11416</v>
+        <v>17.12</v>
       </c>
       <c r="C2" s="16">
         <v>4234</v>
@@ -18735,7 +18760,7 @@
         <v>69</v>
       </c>
       <c r="B3" s="16">
-        <v>11252</v>
+        <v>16.88</v>
       </c>
       <c r="C3" s="16">
         <v>8036</v>
@@ -18746,7 +18771,7 @@
         <v>34</v>
       </c>
       <c r="B4" s="16">
-        <v>100206</v>
+        <v>150.31</v>
       </c>
       <c r="C4" s="16">
         <v>36900</v>
@@ -18757,7 +18782,7 @@
         <v>73</v>
       </c>
       <c r="B5" s="16">
-        <v>31920</v>
+        <v>47.88</v>
       </c>
       <c r="C5" s="16">
         <v>29326</v>
@@ -18768,7 +18793,7 @@
         <v>133</v>
       </c>
       <c r="B6" s="16">
-        <v>5303</v>
+        <v>7.95</v>
       </c>
       <c r="C6" s="16">
         <v>1865</v>
@@ -18779,7 +18804,7 @@
         <v>32</v>
       </c>
       <c r="B7" s="16">
-        <v>22289</v>
+        <v>33.43</v>
       </c>
       <c r="C7" s="16">
         <v>19308</v>
@@ -18790,7 +18815,7 @@
         <v>317</v>
       </c>
       <c r="B8" s="16">
-        <v>8094</v>
+        <v>12.14</v>
       </c>
       <c r="C8" s="17">
         <v>2841</v>
@@ -18801,7 +18826,7 @@
         <v>197</v>
       </c>
       <c r="B9" s="16">
-        <v>16130</v>
+        <v>24.2</v>
       </c>
       <c r="C9" s="16">
         <v>9098</v>
@@ -18812,7 +18837,7 @@
         <v>247</v>
       </c>
       <c r="B10" s="16">
-        <v>30351</v>
+        <v>45.53</v>
       </c>
       <c r="C10" s="16">
         <v>12479</v>
@@ -18823,7 +18848,7 @@
         <v>25</v>
       </c>
       <c r="B11" s="16">
-        <v>49276</v>
+        <v>73.91</v>
       </c>
       <c r="C11" s="16">
         <v>30120</v>
@@ -18834,7 +18859,7 @@
         <v>27</v>
       </c>
       <c r="B12" s="16">
-        <v>22086</v>
+        <v>33.13</v>
       </c>
       <c r="C12" s="16">
         <v>16923</v>
@@ -18845,7 +18870,7 @@
         <v>20</v>
       </c>
       <c r="B13" s="16">
-        <v>16802</v>
+        <v>25.2</v>
       </c>
       <c r="C13" s="16">
         <v>10729</v>
@@ -18856,7 +18881,7 @@
         <v>84</v>
       </c>
       <c r="B14" s="16">
-        <v>33248</v>
+        <v>49.87</v>
       </c>
       <c r="C14" s="16">
         <v>23106</v>
@@ -18867,7 +18892,7 @@
         <v>271</v>
       </c>
       <c r="B15" s="16">
-        <v>7783</v>
+        <v>11.67</v>
       </c>
       <c r="C15" s="17">
         <v>10456</v>
@@ -18878,7 +18903,7 @@
         <v>164</v>
       </c>
       <c r="B16" s="16">
-        <v>11953</v>
+        <v>17.93</v>
       </c>
       <c r="C16" s="16">
         <v>9317</v>
@@ -18889,7 +18914,7 @@
         <v>311</v>
       </c>
       <c r="B17" s="16">
-        <v>18985</v>
+        <v>28.48</v>
       </c>
       <c r="C17" s="16">
         <v>18716</v>
@@ -18900,7 +18925,7 @@
         <v>16</v>
       </c>
       <c r="B18" s="16">
-        <v>51326</v>
+        <v>76.99</v>
       </c>
       <c r="C18" s="16">
         <v>21825</v>
@@ -18911,7 +18936,7 @@
         <v>14</v>
       </c>
       <c r="B19" s="16">
-        <v>70171</v>
+        <v>105.26</v>
       </c>
       <c r="C19" s="16">
         <v>49603</v>
@@ -18928,7 +18953,7 @@
   <sheetPr/>
   <dimension ref="A1:C172"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>

</xml_diff>